<commit_message>
good amount of work on the filtering analysis
</commit_message>
<xml_diff>
--- a/raw_data/phenotype_data.xlsx
+++ b/raw_data/phenotype_data.xlsx
@@ -8,25 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D7CBB68-94E5-E64B-BB25-6CED8BC5B41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE50E7E1-9425-E744-9A00-53C385EF9F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{95A0B606-8E82-AB4B-B901-46781282E7B7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{95A0B606-8E82-AB4B-B901-46781282E7B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$2:$E$123</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$1:$G$50</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$G$51:$G$123</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$G$1:$G$50</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$G$51:$G$123</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">

</xml_diff>

<commit_message>
back calculation and started global model parameterization
</commit_message>
<xml_diff>
--- a/raw_data/phenotype_data.xlsx
+++ b/raw_data/phenotype_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C884DE0-5455-234F-82FF-E394DCF3AD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEEED05-F0E8-404C-82A4-3C8C7EF139A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{95A0B606-8E82-AB4B-B901-46781282E7B7}"/>
+    <workbookView xWindow="19300" yWindow="500" windowWidth="10000" windowHeight="16480" xr2:uid="{95A0B606-8E82-AB4B-B901-46781282E7B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1346,8 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28D9D8A-4BB1-B749-8FD6-F9946088D456}">
   <dimension ref="A1:P140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121:B140"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
worked a lot on the hfc analysis
</commit_message>
<xml_diff>
--- a/raw_data/phenotype_data.xlsx
+++ b/raw_data/phenotype_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SMB_Fitness/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEEED05-F0E8-404C-82A4-3C8C7EF139A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EC7593-F984-B749-979F-7A6055FEDDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19300" yWindow="500" windowWidth="10000" windowHeight="16480" xr2:uid="{95A0B606-8E82-AB4B-B901-46781282E7B7}"/>
+    <workbookView xWindow="-34320" yWindow="500" windowWidth="28800" windowHeight="20740" xr2:uid="{95A0B606-8E82-AB4B-B901-46781282E7B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1346,9 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28D9D8A-4BB1-B749-8FD6-F9946088D456}">
   <dimension ref="A1:P140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4771,10 +4771,10 @@
         <v>139</v>
       </c>
       <c r="D69" s="2">
+        <v>218</v>
+      </c>
+      <c r="E69" s="2">
         <v>202</v>
-      </c>
-      <c r="E69" s="2">
-        <v>218</v>
       </c>
       <c r="F69" s="2">
         <v>120</v>

</xml_diff>